<commit_message>
Add logic for valid and invalid logins
</commit_message>
<xml_diff>
--- a/src/test/java/com/payBox/testData/BoxData.xlsx
+++ b/src/test/java/com/payBox/testData/BoxData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>password</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>emailAddress</t>
+  </si>
+  <si>
+    <t>saif</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,6 +396,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>